<commit_message>
new stats and plots
</commit_message>
<xml_diff>
--- a/model/model_notes.xlsx
+++ b/model/model_notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25420" yWindow="1120" windowWidth="24900" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="25360" yWindow="1120" windowWidth="24900" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="no collective" sheetId="1" r:id="rId1"/>
@@ -209,14 +209,14 @@
     <t>all states flat</t>
   </si>
   <si>
-    <t>all but no</t>
+    <t>no noise is flat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,6 +236,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -7340,7 +7346,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8255,6 +8261,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
finish model, start discussion
</commit_message>
<xml_diff>
--- a/model/model_notes.xlsx
+++ b/model/model_notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25360" yWindow="1120" windowWidth="24900" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView minimized="1" xWindow="25520" yWindow="4480" windowWidth="25020" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="no collective" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="66">
   <si>
     <t>amb</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>no noise is flat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 4 5 </t>
+  </si>
+  <si>
+    <t>heavy</t>
+  </si>
+  <si>
+    <t>p(coll)</t>
   </si>
 </sst>
 </file>
@@ -7343,10 +7352,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7367,7 +7376,7 @@
     <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -7410,8 +7419,11 @@
       <c r="N1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7452,7 +7464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7493,7 +7505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -7534,7 +7546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -7575,7 +7587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -7616,7 +7628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -7657,7 +7669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -7698,7 +7710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -7739,7 +7751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -7780,7 +7792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -7821,7 +7833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -7862,7 +7874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -7903,7 +7915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -7944,7 +7956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -7985,7 +7997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -8258,6 +8270,41 @@
       </c>
       <c r="N22" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>